<commit_message>
dynamic card setting for scenario 1
</commit_message>
<xml_diff>
--- a/gridToFill Iteration 1 Team 11.xlsx
+++ b/gridToFill Iteration 1 Team 11.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gack\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gack\eclipse-workspace\3004Team11\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CE3C0E-E447-4174-9A1A-7C17E20A112F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="4680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -845,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1272,7 +1273,7 @@
         <v>52</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
chenged scenario 1 to the sheet we never saw before
</commit_message>
<xml_diff>
--- a/gridToFill Iteration 1 Team 11.xlsx
+++ b/gridToFill Iteration 1 Team 11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gack\eclipse-workspace\3004Team11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1056A949-0DA2-49F7-8962-972E74E3B021}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F22263-6104-41D0-AC49-8D93A86DF6E0}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="4680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -846,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>